<commit_message>
#110 refactored + demo session notification
</commit_message>
<xml_diff>
--- a/assets/demo/excel/model1.xlsx
+++ b/assets/demo/excel/model1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philipp\Nextcloud\Berufsschule\projekte\untis_phasierung\assets\demo\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E630D733-EAC9-4CEF-9144-64543FA62BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B987AE4C-05CD-485B-8DD4-C2CAEF6E7E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2628" yWindow="2124" windowWidth="9912" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="24">
   <si>
     <t>Stunde</t>
   </si>
@@ -43,30 +43,6 @@
   </si>
   <si>
     <t xml:space="preserve">Freitag </t>
-  </si>
-  <si>
-    <t>DON</t>
-  </si>
-  <si>
-    <t>CAG</t>
-  </si>
-  <si>
-    <t>HEY</t>
-  </si>
-  <si>
-    <t>BEI</t>
-  </si>
-  <si>
-    <t>Gau</t>
-  </si>
-  <si>
-    <t>SCADI</t>
-  </si>
-  <si>
-    <t>RUF</t>
-  </si>
-  <si>
-    <t>FUE</t>
   </si>
   <si>
     <t>Woche 1</t>
@@ -92,6 +68,36 @@
   <si>
     <t>Block 6.12 - 22.12 MODELL</t>
   </si>
+  <si>
+    <t>DOE</t>
+  </si>
+  <si>
+    <t>WAW</t>
+  </si>
+  <si>
+    <t>ETZ</t>
+  </si>
+  <si>
+    <t>KAG</t>
+  </si>
+  <si>
+    <t>MUS</t>
+  </si>
+  <si>
+    <t>LPT</t>
+  </si>
+  <si>
+    <t>SDI</t>
+  </si>
+  <si>
+    <t>DLE</t>
+  </si>
+  <si>
+    <t>LTZ</t>
+  </si>
+  <si>
+    <t>KA</t>
+  </si>
 </sst>
 </file>
 
@@ -114,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +163,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA21FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -194,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -204,7 +216,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -218,6 +229,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -226,6 +240,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFEA21FF"/>
       <color rgb="FFFFFF00"/>
       <color rgb="FFFFC000"/>
     </mruColors>
@@ -506,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BK96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J7"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,25 +532,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="C1" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="2" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C2" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="J2" s="8"/>
+      <c r="C2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
@@ -556,42 +571,42 @@
       <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>16</v>
+      <c r="I3" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="11" t="s">
-        <v>18</v>
+      <c r="I5" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="3:10" x14ac:dyDescent="0.3">
@@ -599,22 +614,22 @@
         <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="3:10" x14ac:dyDescent="0.3">
@@ -622,10 +637,10 @@
       <c r="D7" s="4"/>
       <c r="E7" s="6"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="13" t="s">
-        <v>20</v>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="3:10" x14ac:dyDescent="0.3">
@@ -633,54 +648,52 @@
         <v>3</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="4"/>
       <c r="E9" s="6"/>
-      <c r="F9" s="4"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C10" s="3">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>11</v>
+      <c r="D10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="4"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
@@ -688,60 +701,60 @@
       <c r="C12" s="3">
         <v>5</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>12</v>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="16"/>
       <c r="E13" s="4"/>
       <c r="F13" s="2"/>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C14" s="3">
         <v>6</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>12</v>
+      <c r="D14" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>11</v>
+      <c r="G14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C15" s="3"/>
-      <c r="D15" s="7"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="4"/>
       <c r="F15" s="2"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C16" s="3">
         <v>7</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>12</v>
+      <c r="D16" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -750,7 +763,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C17" s="3"/>
-      <c r="D17" s="7"/>
+      <c r="D17" s="17"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -760,8 +773,8 @@
       <c r="C18" s="3">
         <v>8</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>12</v>
+      <c r="D18" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -772,21 +785,21 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="7"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C22" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
+      <c r="C22" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
@@ -813,180 +826,184 @@
         <v>1</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C25" s="3"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C26" s="3">
         <v>2</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="D26" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C28" s="3">
         <v>3</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C29" s="3"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="4"/>
+      <c r="E29" s="6"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C30" s="3">
         <v>4</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>10</v>
+      <c r="D30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C32" s="3">
         <v>5</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>13</v>
+      <c r="D32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="F32" s="2"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" spans="3:52" x14ac:dyDescent="0.3">
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="E33" s="16"/>
       <c r="F33" s="2"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
     </row>
     <row r="34" spans="3:52" x14ac:dyDescent="0.3">
       <c r="C34" s="3">
         <v>6</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>12</v>
+      <c r="D34" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F34" s="2"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
     </row>
     <row r="35" spans="3:52" x14ac:dyDescent="0.3">
       <c r="C35" s="3"/>
-      <c r="D35" s="7"/>
+      <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="2"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
     </row>
     <row r="36" spans="3:52" x14ac:dyDescent="0.3">
       <c r="C36" s="3">
         <v>7</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>12</v>
+      <c r="D36" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
     </row>
     <row r="37" spans="3:52" x14ac:dyDescent="0.3">
       <c r="C37" s="3"/>
-      <c r="D37" s="7"/>
+      <c r="D37" s="4"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
     </row>
     <row r="38" spans="3:52" x14ac:dyDescent="0.3">
       <c r="C38" s="3">
         <v>8</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>12</v>
+      <c r="D38" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
     </row>
     <row r="39" spans="3:52" x14ac:dyDescent="0.3">
       <c r="C39" s="2"/>
-      <c r="D39" s="7"/>
+      <c r="D39" s="16"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="46" spans="3:52" x14ac:dyDescent="0.3">
       <c r="R46" s="1"/>

</xml_diff>

<commit_message>
#134 fix + color improvement
</commit_message>
<xml_diff>
--- a/assets/demo/excel/model1.xlsx
+++ b/assets/demo/excel/model1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philipp\Nextcloud\Berufsschule\projekte\untis_phasierung\assets\demo\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B987AE4C-05CD-485B-8DD4-C2CAEF6E7E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562552D4-7206-4C0C-81F3-3DF7C7C18E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2628" yWindow="2124" windowWidth="9912" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1344" yWindow="2616" windowWidth="15024" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -206,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -223,15 +223,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -522,7 +523,7 @@
   <dimension ref="A1:BK96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,24 +533,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.3">
@@ -692,7 +693,7 @@
     <row r="11" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C11" s="3"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="16"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="6"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -717,7 +718,7 @@
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C13" s="3"/>
-      <c r="D13" s="16"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="4"/>
       <c r="F13" s="2"/>
       <c r="G13" s="4"/>
@@ -727,7 +728,7 @@
       <c r="C14" s="3">
         <v>6</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -743,7 +744,7 @@
     </row>
     <row r="15" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C15" s="3"/>
-      <c r="D15" s="17"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="4"/>
       <c r="F15" s="2"/>
       <c r="G15" s="4"/>
@@ -753,7 +754,7 @@
       <c r="C16" s="3">
         <v>7</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="2"/>
@@ -763,7 +764,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C17" s="3"/>
-      <c r="D17" s="17"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -773,7 +774,7 @@
       <c r="C18" s="3">
         <v>8</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="2"/>
@@ -785,21 +786,21 @@
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="17"/>
+      <c r="D19" s="15"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
@@ -828,10 +829,10 @@
       <c r="D24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="16" t="s">
         <v>15</v>
       </c>
       <c r="G24" s="13"/>
@@ -840,10 +841,10 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C25" s="3"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="18"/>
+      <c r="F25" s="16"/>
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
     </row>
@@ -857,7 +858,7 @@
       <c r="E26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="16" t="s">
         <v>15</v>
       </c>
       <c r="G26" s="13"/>
@@ -869,7 +870,7 @@
       <c r="E27" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
     </row>
@@ -883,7 +884,7 @@
       <c r="E28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F28" s="5" t="s">
         <v>20</v>
       </c>
       <c r="G28" s="13"/>
@@ -907,7 +908,7 @@
       <c r="E30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="6" t="s">
         <v>20</v>
       </c>
       <c r="G30" s="13"/>
@@ -917,7 +918,7 @@
       <c r="C31" s="3"/>
       <c r="D31" s="6"/>
       <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="F31" s="19"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
     </row>
@@ -938,7 +939,7 @@
     <row r="33" spans="3:52" x14ac:dyDescent="0.3">
       <c r="C33" s="3"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="16"/>
+      <c r="E33" s="14"/>
       <c r="F33" s="2"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
@@ -999,7 +1000,7 @@
     </row>
     <row r="39" spans="3:52" x14ac:dyDescent="0.3">
       <c r="C39" s="2"/>
-      <c r="D39" s="16"/>
+      <c r="D39" s="14"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="13"/>

</xml_diff>